<commit_message>
info: updated regression results from paper
</commit_message>
<xml_diff>
--- a/evaluation/regression/paper results formatted.xlsx
+++ b/evaluation/regression/paper results formatted.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loftuw\Documents\Github\calibrated_explanations\evaluation\regression\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23CAC1D9-B936-459B-AF79-008962BC0087}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3CAC1D1-E606-4572-9D3F-8B411C93C56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{BCF3E74A-1CAB-4D45-9120-A9E677C16434}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" activeTab="3" xr2:uid="{BCF3E74A-1CAB-4D45-9120-A9E677C16434}"/>
   </bookViews>
   <sheets>
     <sheet name="Stability" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="7" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="35">
   <si>
     <t>Stability</t>
   </si>
@@ -146,6 +146,9 @@
   <si>
     <t>CPS</t>
   </si>
+  <si>
+    <t>(Old results below, before remake of core explanation function)</t>
+  </si>
 </sst>
 </file>
 
@@ -197,7 +200,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -283,11 +286,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF999999"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF999999"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -308,7 +331,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
@@ -328,23 +350,49 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" pivotButton="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="99">
+  <dxfs count="144">
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
@@ -352,10 +400,7 @@
       <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
@@ -484,34 +529,262 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode=".000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
     </dxf>
     <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=".0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=".0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=".0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=".0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="15" formatCode="0.00E+00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0E+00"/>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color indexed="64"/>
@@ -546,7 +819,7 @@
       <numFmt numFmtId="164" formatCode="0.0E+00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode=".000"/>
+      <numFmt numFmtId="167" formatCode=".000"/>
     </dxf>
     <dxf>
       <border>
@@ -715,7 +988,7 @@
       <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
@@ -724,84 +997,16 @@
       <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <numFmt numFmtId="165" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center"/>
     </dxf>
     <dxf>
       <font>
@@ -809,6 +1014,86 @@
       </font>
     </dxf>
     <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
       </font>
@@ -844,13 +1129,18 @@
       </font>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.000"/>
@@ -862,13 +1152,13 @@
       <numFmt numFmtId="164" formatCode="0.0E+00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=".0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=".0000"/>
+      <numFmt numFmtId="168" formatCode=".0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=".0000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0E+00"/>
@@ -877,13 +1167,13 @@
       <numFmt numFmtId="15" formatCode="0.00E+00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode=".0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.0000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode=".0000"/>
+      <numFmt numFmtId="168" formatCode=".0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.0000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode=".0000"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -899,7 +1189,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Tuwe Löfström" refreshedDate="45424.019592824072" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="33" xr:uid="{C4CFA6F4-1D22-4081-86BB-5B198F4E18C7}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Tuwe Löfström" refreshedDate="45549.637822222219" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="33" xr:uid="{C4CFA6F4-1D22-4081-86BB-5B198F4E18C7}">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:F1048576" sheet="Sheet1"/>
   </cacheSource>
@@ -927,16 +1217,16 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Stability" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="2.7439999999999999E-34" maxValue="4.2950000000000002E-3"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="6.2109999999999996E-34" maxValue="4.1240000000000001E-3"/>
     </cacheField>
     <cacheField name="Robustness" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.3540000000000001E-4" maxValue="3.9269999999999999E-2"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="1.3630000000000001E-4" maxValue="4.0140000000000002E-2"/>
     </cacheField>
     <cacheField name="Prediction Variance" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="9.0690000000000001E-5" maxValue="9.0690000000000001E-5"/>
     </cacheField>
     <cacheField name="Stability time" numFmtId="0">
-      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.16600000000000001" maxValue="2.7570000000000001"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="3.5000000000000003E-2" maxValue="1.716"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -952,258 +1242,258 @@
   <r>
     <x v="0"/>
     <x v="0"/>
-    <n v="2.7399999999999999E-5"/>
+    <n v="2.957E-5"/>
     <n v="8.8130000000000001E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.16600000000000001"/>
+    <n v="0.13700000000000001"/>
   </r>
   <r>
     <x v="1"/>
     <x v="0"/>
-    <n v="7.9439999999999998E-34"/>
+    <n v="1.7189999999999999E-33"/>
     <n v="1.4249999999999999E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.43099999999999999"/>
+    <n v="0.38300000000000001"/>
   </r>
   <r>
     <x v="0"/>
     <x v="1"/>
-    <n v="2.692E-5"/>
+    <n v="2.919E-5"/>
     <n v="8.7109999999999998E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.188"/>
+    <n v="0.15"/>
   </r>
   <r>
     <x v="0"/>
     <x v="2"/>
-    <n v="2.7460000000000001E-5"/>
-    <n v="8.5139999999999999E-4"/>
+    <n v="2.9240000000000001E-5"/>
+    <n v="8.5329999999999998E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.254"/>
+    <n v="0.223"/>
   </r>
   <r>
     <x v="0"/>
     <x v="3"/>
-    <n v="2.8050000000000001E-5"/>
-    <n v="8.5220000000000001E-4"/>
+    <n v="3.0920000000000002E-5"/>
+    <n v="8.5389999999999999E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.34799999999999998"/>
+    <n v="0.30499999999999999"/>
   </r>
   <r>
     <x v="0"/>
     <x v="4"/>
-    <n v="2.652E-5"/>
-    <n v="8.6410000000000002E-4"/>
+    <n v="2.7840000000000001E-5"/>
+    <n v="8.6589999999999996E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.26500000000000001"/>
+    <n v="0.23"/>
   </r>
   <r>
     <x v="0"/>
     <x v="5"/>
-    <n v="2.2650000000000002E-5"/>
-    <n v="8.8139999999999996E-4"/>
+    <n v="2.4110000000000001E-5"/>
+    <n v="8.8170000000000002E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.29399999999999998"/>
+    <n v="0.25800000000000001"/>
   </r>
   <r>
     <x v="1"/>
     <x v="1"/>
-    <n v="7.8960000000000004E-34"/>
+    <n v="6.2109999999999996E-34"/>
     <n v="1.4249999999999999E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.58699999999999997"/>
+    <n v="0.51700000000000002"/>
   </r>
   <r>
     <x v="1"/>
     <x v="2"/>
-    <n v="2.7439999999999999E-34"/>
+    <n v="7.7039999999999993E-34"/>
     <n v="1.4119999999999999E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.999"/>
+    <n v="0.96699999999999997"/>
   </r>
   <r>
     <x v="1"/>
     <x v="3"/>
-    <n v="8.4740000000000008E-34"/>
-    <n v="1.407E-4"/>
+    <n v="1.1030000000000001E-33"/>
+    <n v="1.4090000000000001E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.9379999999999999"/>
+    <n v="1.716"/>
   </r>
   <r>
     <x v="1"/>
     <x v="4"/>
-    <n v="8.4740000000000008E-34"/>
-    <n v="1.416E-4"/>
+    <n v="8.9070000000000001E-34"/>
+    <n v="1.4190000000000001E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.198"/>
+    <n v="1.1040000000000001"/>
   </r>
   <r>
     <x v="1"/>
     <x v="5"/>
-    <n v="1.5209999999999999E-33"/>
-    <n v="1.3540000000000001E-4"/>
+    <n v="7.5109999999999996E-34"/>
+    <n v="1.3630000000000001E-4"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.1870000000000001"/>
+    <n v="1.056"/>
   </r>
   <r>
     <x v="2"/>
     <x v="1"/>
-    <n v="8.9359999999999997E-33"/>
+    <n v="1.9719999999999999E-32"/>
     <n v="8.0110000000000008E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.26900000000000002"/>
+    <n v="3.5000000000000003E-2"/>
   </r>
   <r>
     <x v="2"/>
     <x v="2"/>
-    <n v="9.5530000000000003E-33"/>
+    <n v="1.5409999999999999E-32"/>
     <n v="7.7460000000000003E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.728"/>
+    <n v="9.7000000000000003E-2"/>
   </r>
   <r>
     <x v="2"/>
     <x v="3"/>
-    <n v="7.396E-33"/>
+    <n v="9.5530000000000003E-33"/>
     <n v="7.8510000000000003E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.7989999999999999"/>
+    <n v="0.17299999999999999"/>
   </r>
   <r>
     <x v="2"/>
     <x v="4"/>
-    <n v="1.1400000000000001E-32"/>
+    <n v="1.079E-32"/>
     <n v="7.8919999999999997E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.849"/>
+    <n v="0.23400000000000001"/>
   </r>
   <r>
     <x v="2"/>
     <x v="5"/>
-    <n v="8.0119999999999999E-33"/>
+    <n v="1.7560000000000001E-32"/>
     <n v="7.2789999999999999E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.0049999999999999"/>
+    <n v="0.32800000000000001"/>
   </r>
   <r>
     <x v="3"/>
     <x v="1"/>
-    <n v="2.0410000000000001E-33"/>
+    <n v="2.1760000000000002E-33"/>
     <n v="2.0539999999999998E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.4"/>
+    <n v="6.3E-2"/>
   </r>
   <r>
     <x v="3"/>
     <x v="2"/>
-    <n v="2.215E-33"/>
+    <n v="2.5040000000000001E-33"/>
     <n v="2.0010000000000002E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="2.452"/>
+    <n v="0.13700000000000001"/>
   </r>
   <r>
     <x v="3"/>
     <x v="3"/>
-    <n v="3.0429999999999999E-33"/>
+    <n v="1.6369999999999999E-33"/>
     <n v="2.042E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="2.5339999999999998"/>
+    <n v="0.21099999999999999"/>
   </r>
   <r>
     <x v="3"/>
     <x v="4"/>
-    <n v="1.8100000000000001E-33"/>
+    <n v="2.812E-33"/>
     <n v="2.0309999999999998E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="2.613"/>
+    <n v="0.308"/>
   </r>
   <r>
     <x v="3"/>
     <x v="5"/>
-    <n v="5.7780000000000003E-34"/>
+    <n v="1.9070000000000001E-33"/>
     <n v="1.812E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.39"/>
+    <n v="0.36099999999999999"/>
   </r>
   <r>
     <x v="4"/>
     <x v="1"/>
-    <n v="2.2200000000000002E-3"/>
-    <n v="3.4270000000000002E-2"/>
+    <n v="2.7360000000000002E-3"/>
+    <n v="3.465E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.61399999999999999"/>
+    <n v="6.6000000000000003E-2"/>
   </r>
   <r>
     <x v="4"/>
     <x v="2"/>
-    <n v="3.1359999999999999E-3"/>
-    <n v="2.9610000000000001E-2"/>
+    <n v="3.5999999999999999E-3"/>
+    <n v="3.023E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.8380000000000001"/>
+    <n v="0.14899999999999999"/>
   </r>
   <r>
     <x v="4"/>
     <x v="3"/>
-    <n v="2.2239999999999998E-3"/>
-    <n v="3.8109999999999998E-2"/>
+    <n v="2.7560000000000002E-3"/>
+    <n v="3.8449999999999998E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.8839999999999999"/>
+    <n v="0.23"/>
   </r>
   <r>
     <x v="4"/>
     <x v="4"/>
-    <n v="2.3730000000000001E-3"/>
-    <n v="3.9269999999999999E-2"/>
+    <n v="2.689E-3"/>
+    <n v="4.0140000000000002E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.954"/>
+    <n v="0.28899999999999998"/>
   </r>
   <r>
     <x v="4"/>
     <x v="5"/>
-    <n v="2.3400000000000001E-3"/>
-    <n v="3.0929999999999999E-2"/>
+    <n v="2.921E-3"/>
+    <n v="3.116E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.456"/>
+    <n v="0.371"/>
   </r>
   <r>
     <x v="5"/>
     <x v="1"/>
-    <n v="2.6719999999999999E-3"/>
-    <n v="1.259E-2"/>
+    <n v="2.555E-3"/>
+    <n v="1.2319999999999999E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="0.88"/>
+    <n v="9.4E-2"/>
   </r>
   <r>
     <x v="5"/>
     <x v="2"/>
-    <n v="2.7490000000000001E-3"/>
-    <n v="1.128E-2"/>
+    <n v="2.7320000000000001E-3"/>
+    <n v="1.1730000000000001E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="2.64"/>
+    <n v="0.17799999999999999"/>
   </r>
   <r>
     <x v="5"/>
     <x v="3"/>
-    <n v="2.0990000000000002E-3"/>
-    <n v="1.438E-2"/>
+    <n v="2.0660000000000001E-3"/>
+    <n v="1.519E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="2.6909999999999998"/>
+    <n v="0.255"/>
   </r>
   <r>
     <x v="5"/>
     <x v="4"/>
-    <n v="2.2920000000000002E-3"/>
-    <n v="1.5720000000000001E-2"/>
+    <n v="2.0730000000000002E-3"/>
+    <n v="1.5859999999999999E-2"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="2.7570000000000001"/>
+    <n v="0.32200000000000001"/>
   </r>
   <r>
     <x v="5"/>
     <x v="5"/>
-    <n v="4.2950000000000002E-3"/>
-    <n v="9.9760000000000005E-3"/>
+    <n v="4.1240000000000001E-3"/>
+    <n v="9.3150000000000004E-3"/>
     <n v="9.0690000000000001E-5"/>
-    <n v="1.962"/>
+    <n v="0.39600000000000002"/>
   </r>
   <r>
     <x v="6"/>
@@ -1217,7 +1507,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A42D52D-9FFD-405B-9311-A2356325C1A8}" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6A42D52D-9FFD-405B-9311-A2356325C1A8}" name="PivotTable1" cacheId="7" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:G11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -1302,7 +1592,7 @@
     <dataField name="Stability " fld="2" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="5">
-    <format dxfId="98">
+    <format dxfId="143">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1317,7 +1607,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="97">
+    <format dxfId="142">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1326,7 +1616,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="96">
+    <format dxfId="141">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1335,10 +1625,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="95">
+    <format dxfId="140">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="94">
+    <format dxfId="139">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1355,7 +1645,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F1559B5-A5A0-4AE6-9DFE-1FC78E0406E8}" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8F1559B5-A5A0-4AE6-9DFE-1FC78E0406E8}" name="PivotTable1" cacheId="7" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:H11" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -1443,7 +1733,7 @@
     <dataField name="Robustness " fld="3" subtotal="average" baseField="0" baseItem="0" numFmtId="164"/>
   </dataFields>
   <formats count="4">
-    <format dxfId="93">
+    <format dxfId="138">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1458,7 +1748,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="92">
+    <format dxfId="137">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1467,7 +1757,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="91">
+    <format dxfId="136">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1476,7 +1766,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="90">
+    <format dxfId="135">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1493,7 +1783,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A8831D0-ABA7-454A-8E19-32E60F750F56}" name="PivotTable1" cacheId="0" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Normalization" colHeaderCaption="Explanations">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2A8831D0-ABA7-454A-8E19-32E60F750F56}" name="PivotTable1" cacheId="7" dataPosition="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Normalization" colHeaderCaption="Explanations">
   <location ref="A3:F10" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0">
@@ -1572,7 +1862,7 @@
     <dataField name="Time " fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="89">
+    <format dxfId="134">
       <pivotArea field="0" grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1582,7 +1872,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="88">
+    <format dxfId="133">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1592,7 +1882,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="87">
+    <format dxfId="132">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1601,7 +1891,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="86">
+    <format dxfId="131">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1610,16 +1900,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="85">
+    <format dxfId="130">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="84">
+    <format dxfId="129">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="83">
+    <format dxfId="128">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="82">
+    <format dxfId="127">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="4">
@@ -1631,80 +1921,80 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="81">
+    <format dxfId="126">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="80">
+    <format dxfId="125">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="79">
+    <format dxfId="124">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="78">
+    <format dxfId="123">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="77">
+    <format dxfId="122">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="76">
+    <format dxfId="121">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="75">
+    <format dxfId="120">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="74">
+    <format dxfId="119">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="73">
+    <format dxfId="118">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="72">
+    <format dxfId="117">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="71">
+    <format dxfId="116">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="70">
+    <format dxfId="115">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="69">
+    <format dxfId="114">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="68">
+    <format dxfId="113">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="67">
+    <format dxfId="112">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="31">
+    <format dxfId="111">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="30">
+    <format dxfId="110">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="29">
+    <format dxfId="109">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="108">
       <pivotArea dataOnly="0" labelOnly="1" grandCol="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="0">
+    <format dxfId="107">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
   </formats>
@@ -1721,7 +2011,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A40A2CF-E4A8-49E8-AF45-684EEDE25CFF}" name="PivotTable1" cacheId="0" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Normalization" colHeaderCaption="Explanations">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{0A40A2CF-E4A8-49E8-AF45-684EEDE25CFF}" name="PivotTable1" cacheId="7" dataOnRows="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" grandTotalCaption="Average" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" rowHeaderCaption="Normalization" colHeaderCaption="Explanations">
   <location ref="A3:I8" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="6">
     <pivotField axis="axisCol" showAll="0" defaultSubtotal="0">
@@ -1808,7 +2098,7 @@
     <dataField name="Time " fld="5" subtotal="average" baseField="0" baseItem="0" numFmtId="2"/>
   </dataFields>
   <formats count="35">
-    <format dxfId="66">
+    <format dxfId="106">
       <pivotArea field="0" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1818,7 +2108,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="65">
+    <format dxfId="105">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -1828,7 +2118,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="64">
+    <format dxfId="104">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1837,7 +2127,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="63">
+    <format dxfId="103">
       <pivotArea field="0" grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" axis="axisCol" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
@@ -1846,16 +2136,16 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="62">
+    <format dxfId="102">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="61">
+    <format dxfId="101">
       <pivotArea grandCol="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="60">
+    <format dxfId="100">
       <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="59">
+    <format dxfId="99">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="4">
@@ -1867,47 +2157,47 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="58">
+    <format dxfId="98">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="57">
+    <format dxfId="97">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="56">
+    <format dxfId="96">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="55">
+    <format dxfId="95">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="54">
+    <format dxfId="94">
       <pivotArea dataOnly="0" labelOnly="1" grandRow="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="93">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="92">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="91">
       <pivotArea type="origin" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="50">
+    <format dxfId="90">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="49">
+    <format dxfId="89">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="1"/>
     </format>
-    <format dxfId="48">
+    <format dxfId="88">
       <pivotArea type="topRight" dataOnly="0" labelOnly="1" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="87">
       <pivotArea field="-2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="86">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -1918,14 +2208,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="85">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="44">
+    <format dxfId="84">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -1937,7 +2227,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="43">
+    <format dxfId="83">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -1949,7 +2239,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="82">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -1961,7 +2251,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="41">
+    <format dxfId="81">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -1973,7 +2263,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="40">
+    <format dxfId="80">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -1983,7 +2273,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="39">
+    <format dxfId="79">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -1993,10 +2283,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="78">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="37">
+    <format dxfId="77">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="2">
@@ -2006,7 +2296,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="36">
+    <format dxfId="76">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1">
@@ -2015,7 +2305,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="35">
+    <format dxfId="75">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -2027,10 +2317,10 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="74">
       <pivotArea field="0" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisCol" fieldPosition="0"/>
     </format>
-    <format dxfId="33">
+    <format dxfId="73">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="1">
           <reference field="0" count="1">
@@ -2039,7 +2329,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="72">
       <pivotArea dataOnly="0" labelOnly="1" fieldPosition="0">
         <references count="2">
           <reference field="0" count="1" selected="0">
@@ -2387,26 +2677,26 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>19</v>
       </c>
@@ -2414,7 +2704,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -2437,7 +2727,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -2446,148 +2736,148 @@
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7">
-        <v>2.7399999999999999E-5</v>
+        <v>2.957E-5</v>
       </c>
       <c r="G5" s="7">
-        <v>7.9439999999999998E-34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.7189999999999999E-33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="7">
-        <v>8.9359999999999997E-33</v>
+        <v>1.9719999999999999E-32</v>
       </c>
       <c r="C6" s="7">
-        <v>2.0410000000000001E-33</v>
+        <v>2.1760000000000002E-33</v>
       </c>
       <c r="D6" s="7">
-        <v>2.2200000000000002E-3</v>
+        <v>2.7360000000000002E-3</v>
       </c>
       <c r="E6" s="7">
-        <v>2.6719999999999999E-3</v>
+        <v>2.555E-3</v>
       </c>
       <c r="F6" s="7">
-        <v>2.692E-5</v>
+        <v>2.919E-5</v>
       </c>
       <c r="G6" s="7">
-        <v>7.8960000000000004E-34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+        <v>6.2109999999999996E-34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="7">
-        <v>9.5530000000000003E-33</v>
+        <v>1.5409999999999999E-32</v>
       </c>
       <c r="C7" s="7">
-        <v>2.215E-33</v>
+        <v>2.5040000000000001E-33</v>
       </c>
       <c r="D7" s="7">
-        <v>3.1359999999999999E-3</v>
+        <v>3.5999999999999999E-3</v>
       </c>
       <c r="E7" s="7">
-        <v>2.7490000000000001E-3</v>
+        <v>2.7320000000000001E-3</v>
       </c>
       <c r="F7" s="7">
-        <v>2.7460000000000001E-5</v>
+        <v>2.9240000000000001E-5</v>
       </c>
       <c r="G7" s="7">
-        <v>2.7439999999999999E-34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7.7039999999999993E-34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="7">
-        <v>7.396E-33</v>
+        <v>9.5530000000000003E-33</v>
       </c>
       <c r="C8" s="7">
-        <v>3.0429999999999999E-33</v>
+        <v>1.6369999999999999E-33</v>
       </c>
       <c r="D8" s="7">
-        <v>2.2239999999999998E-3</v>
+        <v>2.7560000000000002E-3</v>
       </c>
       <c r="E8" s="7">
-        <v>2.0990000000000002E-3</v>
+        <v>2.0660000000000001E-3</v>
       </c>
       <c r="F8" s="7">
-        <v>2.8050000000000001E-5</v>
+        <v>3.0920000000000002E-5</v>
       </c>
       <c r="G8" s="7">
-        <v>8.4740000000000008E-34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+        <v>1.1030000000000001E-33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="7">
-        <v>1.1400000000000001E-32</v>
+        <v>1.079E-32</v>
       </c>
       <c r="C9" s="7">
-        <v>1.8100000000000001E-33</v>
+        <v>2.812E-33</v>
       </c>
       <c r="D9" s="7">
-        <v>2.3730000000000001E-3</v>
+        <v>2.689E-3</v>
       </c>
       <c r="E9" s="7">
-        <v>2.2920000000000002E-3</v>
+        <v>2.0730000000000002E-3</v>
       </c>
       <c r="F9" s="7">
-        <v>2.652E-5</v>
+        <v>2.7840000000000001E-5</v>
       </c>
       <c r="G9" s="7">
-        <v>8.4740000000000008E-34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+        <v>8.9070000000000001E-34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="7">
-        <v>8.0119999999999999E-33</v>
+        <v>1.7560000000000001E-32</v>
       </c>
       <c r="C10" s="7">
-        <v>5.7780000000000003E-34</v>
+        <v>1.9070000000000001E-33</v>
       </c>
       <c r="D10" s="7">
-        <v>2.3400000000000001E-3</v>
+        <v>2.921E-3</v>
       </c>
       <c r="E10" s="7">
-        <v>4.2950000000000002E-3</v>
+        <v>4.1240000000000001E-3</v>
       </c>
       <c r="F10" s="7">
-        <v>2.2650000000000002E-5</v>
+        <v>2.4110000000000001E-5</v>
       </c>
       <c r="G10" s="7">
-        <v>1.5209999999999999E-33</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+        <v>7.5109999999999996E-34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
       <c r="B11" s="7">
-        <v>9.0594000000000001E-33</v>
+        <v>1.4606600000000001E-32</v>
       </c>
       <c r="C11" s="7">
-        <v>1.9373599999999999E-33</v>
+        <v>2.2072000000000001E-33</v>
       </c>
       <c r="D11" s="7">
-        <v>2.4586E-3</v>
+        <v>2.9404000000000001E-3</v>
       </c>
       <c r="E11" s="7">
-        <v>2.8214000000000004E-3</v>
+        <v>2.7099999999999997E-3</v>
       </c>
       <c r="F11" s="7">
-        <v>2.6500000000000004E-5</v>
+        <v>2.8478333333333338E-5</v>
       </c>
       <c r="G11" s="7">
-        <v>8.4569999999999993E-34</v>
+        <v>9.7588333333333335E-34</v>
       </c>
     </row>
   </sheetData>
@@ -2603,26 +2893,26 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>20</v>
       </c>
@@ -2630,7 +2920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>18</v>
       </c>
@@ -2656,7 +2946,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>31</v>
       </c>
@@ -2674,7 +2964,7 @@
         <v>5.1190000000000003E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>13</v>
       </c>
@@ -2685,10 +2975,10 @@
         <v>2.0539999999999998E-3</v>
       </c>
       <c r="D6" s="7">
-        <v>3.4270000000000002E-2</v>
+        <v>3.465E-2</v>
       </c>
       <c r="E6" s="7">
-        <v>1.259E-2</v>
+        <v>1.2319999999999999E-2</v>
       </c>
       <c r="F6" s="7">
         <v>8.7109999999999998E-4</v>
@@ -2697,10 +2987,10 @@
         <v>1.4249999999999999E-4</v>
       </c>
       <c r="H6" s="7">
-        <v>9.6564333333333339E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+        <v>9.6747666666666659E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
@@ -2711,22 +3001,22 @@
         <v>2.0010000000000002E-3</v>
       </c>
       <c r="D7" s="7">
-        <v>2.9610000000000001E-2</v>
+        <v>3.023E-2</v>
       </c>
       <c r="E7" s="7">
-        <v>1.128E-2</v>
+        <v>1.1730000000000001E-2</v>
       </c>
       <c r="F7" s="7">
-        <v>8.5139999999999999E-4</v>
+        <v>8.5329999999999998E-4</v>
       </c>
       <c r="G7" s="7">
         <v>1.4119999999999999E-4</v>
       </c>
       <c r="H7" s="7">
-        <v>8.6049333333333335E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8.7835833333333342E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>10</v>
       </c>
@@ -2737,22 +3027,22 @@
         <v>2.042E-3</v>
       </c>
       <c r="D8" s="7">
-        <v>3.8109999999999998E-2</v>
+        <v>3.8449999999999998E-2</v>
       </c>
       <c r="E8" s="7">
-        <v>1.438E-2</v>
+        <v>1.519E-2</v>
       </c>
       <c r="F8" s="7">
-        <v>8.5220000000000001E-4</v>
+        <v>8.5389999999999999E-4</v>
       </c>
       <c r="G8" s="7">
-        <v>1.407E-4</v>
+        <v>1.4090000000000001E-4</v>
       </c>
       <c r="H8" s="7">
-        <v>1.0562649999999998E-2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.0754633333333333E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>11</v>
       </c>
@@ -2763,22 +3053,22 @@
         <v>2.0309999999999998E-3</v>
       </c>
       <c r="D9" s="7">
-        <v>3.9269999999999999E-2</v>
+        <v>4.0140000000000002E-2</v>
       </c>
       <c r="E9" s="7">
-        <v>1.5720000000000001E-2</v>
+        <v>1.5859999999999999E-2</v>
       </c>
       <c r="F9" s="7">
-        <v>8.6410000000000002E-4</v>
+        <v>8.6589999999999996E-4</v>
       </c>
       <c r="G9" s="7">
-        <v>1.416E-4</v>
+        <v>1.4190000000000001E-4</v>
       </c>
       <c r="H9" s="7">
-        <v>1.0986450000000002E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+        <v>1.1155133333333336E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>12</v>
       </c>
@@ -2789,22 +3079,22 @@
         <v>1.812E-3</v>
       </c>
       <c r="D10" s="7">
-        <v>3.0929999999999999E-2</v>
+        <v>3.116E-2</v>
       </c>
       <c r="E10" s="7">
-        <v>9.9760000000000005E-3</v>
+        <v>9.3150000000000004E-3</v>
       </c>
       <c r="F10" s="7">
-        <v>8.8139999999999996E-4</v>
+        <v>8.8170000000000002E-4</v>
       </c>
       <c r="G10" s="7">
-        <v>1.3540000000000001E-4</v>
+        <v>1.3630000000000001E-4</v>
       </c>
       <c r="H10" s="7">
-        <v>8.5022999999999991E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+        <v>8.4306666666666662E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>17</v>
       </c>
@@ -2815,19 +3105,19 @@
         <v>1.9879999999999997E-3</v>
       </c>
       <c r="D11" s="7">
-        <v>3.4438000000000003E-2</v>
+        <v>3.4925999999999999E-2</v>
       </c>
       <c r="E11" s="7">
-        <v>1.2789200000000001E-2</v>
+        <v>1.2883E-2</v>
       </c>
       <c r="F11" s="7">
-        <v>8.6691666666666677E-4</v>
+        <v>8.6786666666666655E-4</v>
       </c>
       <c r="G11" s="7">
-        <v>1.4065E-4</v>
+        <v>1.4088333333333333E-4</v>
       </c>
       <c r="H11" s="7">
-        <v>9.0906375000000001E-3</v>
+        <v>9.1817656250000011E-3</v>
       </c>
     </row>
   </sheetData>
@@ -2843,185 +3133,188 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.140625" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17.33203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="C3" s="31"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="34" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="31" t="s">
+      <c r="E4" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="34" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="30" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="32">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="C5" s="32">
-        <v>0.4</v>
-      </c>
-      <c r="D5" s="32">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="E5" s="32">
-        <v>0.88</v>
-      </c>
-      <c r="F5" s="33">
-        <v>0.54074999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="35">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="C5" s="35">
+        <v>6.3E-2</v>
+      </c>
+      <c r="D5" s="35">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="E5" s="35">
+        <v>9.4E-2</v>
+      </c>
+      <c r="F5" s="36">
+        <v>6.4500000000000002E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="30" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="32">
-        <v>1.728</v>
-      </c>
-      <c r="C6" s="32">
-        <v>2.452</v>
-      </c>
-      <c r="D6" s="32">
-        <v>1.8380000000000001</v>
-      </c>
-      <c r="E6" s="32">
-        <v>2.64</v>
-      </c>
-      <c r="F6" s="33">
-        <v>2.1644999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B6" s="37">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="C6" s="37">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="D6" s="37">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E6" s="37">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="F6" s="38">
+        <v>0.14024999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="32">
-        <v>1.7989999999999999</v>
-      </c>
-      <c r="C7" s="32">
-        <v>2.5339999999999998</v>
-      </c>
-      <c r="D7" s="32">
-        <v>1.8839999999999999</v>
-      </c>
-      <c r="E7" s="32">
-        <v>2.6909999999999998</v>
-      </c>
-      <c r="F7" s="33">
-        <v>2.2270000000000003</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B7" s="37">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="C7" s="37">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="D7" s="37">
+        <v>0.23</v>
+      </c>
+      <c r="E7" s="37">
+        <v>0.255</v>
+      </c>
+      <c r="F7" s="38">
+        <v>0.21725</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="32">
-        <v>1.849</v>
-      </c>
-      <c r="C8" s="32">
-        <v>2.613</v>
-      </c>
-      <c r="D8" s="32">
-        <v>1.954</v>
-      </c>
-      <c r="E8" s="32">
-        <v>2.7570000000000001</v>
-      </c>
-      <c r="F8" s="33">
-        <v>2.29325</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B8" s="37">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="C8" s="37">
+        <v>0.308</v>
+      </c>
+      <c r="D8" s="37">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="E8" s="37">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="F8" s="38">
+        <v>0.28825000000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="32">
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="C9" s="32">
-        <v>1.39</v>
-      </c>
-      <c r="D9" s="32">
-        <v>1.456</v>
-      </c>
-      <c r="E9" s="32">
-        <v>1.962</v>
-      </c>
-      <c r="F9" s="33">
-        <v>1.4532499999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="30" t="s">
+      <c r="B9" s="37">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="D9" s="37">
+        <v>0.371</v>
+      </c>
+      <c r="E9" s="37">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="F9" s="38">
+        <v>0.36399999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="B10" s="33">
-        <v>1.3299999999999998</v>
-      </c>
-      <c r="C10" s="33">
-        <v>1.8777999999999999</v>
-      </c>
-      <c r="D10" s="33">
-        <v>1.5492000000000001</v>
-      </c>
-      <c r="E10" s="33">
-        <v>2.1859999999999999</v>
-      </c>
-      <c r="F10" s="33">
-        <v>1.7357500000000001</v>
+      <c r="B10" s="39">
+        <v>0.1734</v>
+      </c>
+      <c r="C10" s="39">
+        <v>0.21600000000000003</v>
+      </c>
+      <c r="D10" s="39">
+        <v>0.221</v>
+      </c>
+      <c r="E10" s="39">
+        <v>0.24900000000000003</v>
+      </c>
+      <c r="F10" s="40">
+        <v>0.21485000000000004</v>
       </c>
       <c r="G10"/>
       <c r="H10"/>
       <c r="I10"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="F11"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="F12"/>
     </row>
@@ -3035,198 +3328,202 @@
   <dimension ref="A3:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.6640625" style="9" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.44140625" style="9" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.85546875" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="24" width="21" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="26.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="9" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="14" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="9" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="14" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="7.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="15" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="33"/>
+      <c r="B3" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="21"/>
-      <c r="B4" s="16" t="s">
+      <c r="C3" s="33"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="20"/>
+      <c r="B4" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="23" t="s">
+      <c r="E4" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="24" t="s">
+      <c r="F4" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="20"/>
-      <c r="H4" s="24" t="s">
+      <c r="G4" s="19"/>
+      <c r="H4" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="20"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="I4" s="19"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="B5" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="9" t="s">
+      <c r="C5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="9" t="s">
+      <c r="H5" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="I5" s="33" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="17">
-        <v>8.9359999999999997E-33</v>
-      </c>
-      <c r="C6" s="25">
-        <v>2.0410000000000001E-33</v>
-      </c>
-      <c r="D6" s="25">
-        <v>2.2200000000000002E-3</v>
-      </c>
-      <c r="E6" s="25">
-        <v>2.6719999999999999E-3</v>
-      </c>
-      <c r="F6" s="25">
-        <v>2.7399999999999999E-5</v>
-      </c>
-      <c r="G6" s="7">
-        <v>2.692E-5</v>
-      </c>
-      <c r="H6" s="25">
-        <v>7.9439999999999998E-34</v>
-      </c>
-      <c r="I6" s="7">
-        <v>7.8960000000000004E-34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="22" t="s">
+      <c r="B6" s="16">
+        <v>1.9719999999999999E-32</v>
+      </c>
+      <c r="C6" s="24">
+        <v>2.1760000000000002E-33</v>
+      </c>
+      <c r="D6" s="24">
+        <v>2.7360000000000002E-3</v>
+      </c>
+      <c r="E6" s="24">
+        <v>2.555E-3</v>
+      </c>
+      <c r="F6" s="24">
+        <v>2.957E-5</v>
+      </c>
+      <c r="G6" s="43">
+        <v>2.919E-5</v>
+      </c>
+      <c r="H6" s="24">
+        <v>1.7189999999999999E-33</v>
+      </c>
+      <c r="I6" s="43">
+        <v>6.2109999999999996E-34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="28">
+      <c r="B7" s="27">
         <v>8.0110000000000008E-3</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="26">
         <v>2.0539999999999998E-3</v>
       </c>
-      <c r="D7" s="27">
-        <v>3.4270000000000002E-2</v>
-      </c>
-      <c r="E7" s="27">
-        <v>1.259E-2</v>
-      </c>
-      <c r="F7" s="27">
+      <c r="D7" s="26">
+        <v>3.465E-2</v>
+      </c>
+      <c r="E7" s="26">
+        <v>1.2319999999999999E-2</v>
+      </c>
+      <c r="F7" s="26">
         <v>8.8130000000000001E-4</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="25">
         <v>8.7109999999999998E-4</v>
       </c>
-      <c r="H7" s="27">
+      <c r="H7" s="26">
         <v>1.4249999999999999E-4</v>
       </c>
-      <c r="I7" s="26">
+      <c r="I7" s="25">
         <v>1.4249999999999999E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="22" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="B8" s="29">
-        <v>0.26900000000000002</v>
+      <c r="B8" s="28">
+        <v>3.5000000000000003E-2</v>
       </c>
       <c r="C8" s="10">
-        <v>0.4</v>
+        <v>6.3E-2</v>
       </c>
       <c r="D8" s="10">
-        <v>0.61399999999999999</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="E8" s="10">
-        <v>0.88</v>
+        <v>9.4E-2</v>
       </c>
       <c r="F8" s="10">
-        <v>0.16600000000000001</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="G8" s="11">
-        <v>0.188</v>
+        <v>0.15</v>
       </c>
       <c r="H8" s="10">
-        <v>0.43099999999999999</v>
+        <v>0.38300000000000001</v>
       </c>
       <c r="I8" s="11">
-        <v>0.58699999999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9"/>
+        <v>0.51700000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="44" t="s">
+        <v>34</v>
+      </c>
       <c r="B9"/>
       <c r="F9"/>
     </row>
-    <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10"/>
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>3</v>
       </c>
       <c r="C10" s="9" t="s">
@@ -3251,25 +3548,25 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="19"/>
-      <c r="C11" s="14"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="14"/>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14" t="s">
+    <row r="11" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="18"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14" t="s">
+      <c r="H11" s="13"/>
+      <c r="I11" s="13" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>8.9359999999999997E-33</v>
       </c>
       <c r="C12" s="7">
@@ -3294,11 +3591,11 @@
         <v>7.8960000000000004E-34</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="16">
         <v>8.0110000000000008E-3</v>
       </c>
       <c r="C13" s="7">
@@ -3323,11 +3620,11 @@
         <v>1.4249999999999999E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14" s="18">
+      <c r="B14" s="17">
         <v>0.26900000000000002</v>
       </c>
       <c r="C14" s="10">
@@ -3354,6 +3651,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -3362,38 +3660,43 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:P1048576"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="1"/>
-    <col min="2" max="2" width="8.88671875"/>
-    <col min="3" max="10" width="9.109375" style="1"/>
-    <col min="11" max="11" width="8.88671875" customWidth="1"/>
-    <col min="12" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="9.140625" style="1"/>
+    <col min="11" max="11" width="8.85546875" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="67.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
       <c r="L1" s="2"/>
@@ -3402,27 +3705,27 @@
       <c r="O1" s="2"/>
       <c r="P1" s="2"/>
     </row>
-    <row r="2" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="4">
-        <v>2.7399999999999999E-5</v>
-      </c>
-      <c r="D2" s="4">
+      <c r="C2">
+        <v>2.957E-5</v>
+      </c>
+      <c r="D2">
         <v>8.8130000000000001E-4</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F2" s="3">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="G2" s="3">
-        <v>0.186</v>
+      <c r="F2">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G2">
+        <v>0.16200000000000001</v>
       </c>
       <c r="J2" s="3"/>
       <c r="L2" s="4"/>
@@ -3431,27 +3734,27 @@
       <c r="O2" s="3"/>
       <c r="P2" s="3"/>
     </row>
-    <row r="3" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
       </c>
-      <c r="C3" s="4">
-        <v>7.9439999999999998E-34</v>
-      </c>
-      <c r="D3" s="4">
+      <c r="C3">
+        <v>1.7189999999999999E-33</v>
+      </c>
+      <c r="D3">
         <v>1.4249999999999999E-4</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F3" s="3">
-        <v>0.43099999999999999</v>
-      </c>
-      <c r="G3" s="3">
-        <v>0.45500000000000002</v>
+      <c r="F3">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.39100000000000001</v>
       </c>
       <c r="J3" s="3"/>
       <c r="L3" s="4"/>
@@ -3460,27 +3763,27 @@
       <c r="O3" s="3"/>
       <c r="P3" s="3"/>
     </row>
-    <row r="4" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="4">
-        <v>2.692E-5</v>
-      </c>
-      <c r="D4" s="4">
+      <c r="C4">
+        <v>2.919E-5</v>
+      </c>
+      <c r="D4">
         <v>8.7109999999999998E-4</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F4" s="3">
-        <v>0.188</v>
-      </c>
-      <c r="G4" s="3">
-        <v>0.20699999999999999</v>
+      <c r="F4">
+        <v>0.15</v>
+      </c>
+      <c r="G4">
+        <v>0.16200000000000001</v>
       </c>
       <c r="J4" s="3"/>
       <c r="L4" s="4"/>
@@ -3489,27 +3792,27 @@
       <c r="O4" s="3"/>
       <c r="P4" s="3"/>
     </row>
-    <row r="5" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="4">
-        <v>2.7460000000000001E-5</v>
-      </c>
-      <c r="D5" s="4">
-        <v>8.5139999999999999E-4</v>
-      </c>
-      <c r="E5" s="4">
+      <c r="C5">
+        <v>2.9240000000000001E-5</v>
+      </c>
+      <c r="D5">
+        <v>8.5329999999999998E-4</v>
+      </c>
+      <c r="E5">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F5" s="3">
-        <v>0.254</v>
-      </c>
-      <c r="G5" s="3">
-        <v>0.28699999999999998</v>
+      <c r="F5">
+        <v>0.223</v>
+      </c>
+      <c r="G5">
+        <v>0.24099999999999999</v>
       </c>
       <c r="J5" s="3"/>
       <c r="L5" s="4"/>
@@ -3518,27 +3821,27 @@
       <c r="O5" s="3"/>
       <c r="P5" s="3"/>
     </row>
-    <row r="6" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="4">
-        <v>2.8050000000000001E-5</v>
-      </c>
-      <c r="D6" s="4">
-        <v>8.5220000000000001E-4</v>
-      </c>
-      <c r="E6" s="4">
+      <c r="C6">
+        <v>3.0920000000000002E-5</v>
+      </c>
+      <c r="D6">
+        <v>8.5389999999999999E-4</v>
+      </c>
+      <c r="E6">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F6" s="3">
-        <v>0.34799999999999998</v>
-      </c>
-      <c r="G6" s="3">
-        <v>0.374</v>
+      <c r="F6">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.33100000000000002</v>
       </c>
       <c r="J6" s="3"/>
       <c r="L6" s="4"/>
@@ -3547,27 +3850,27 @@
       <c r="O6" s="3"/>
       <c r="P6" s="3"/>
     </row>
-    <row r="7" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B7" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4">
-        <v>2.652E-5</v>
-      </c>
-      <c r="D7" s="4">
-        <v>8.6410000000000002E-4</v>
-      </c>
-      <c r="E7" s="4">
+      <c r="C7">
+        <v>2.7840000000000001E-5</v>
+      </c>
+      <c r="D7">
+        <v>8.6589999999999996E-4</v>
+      </c>
+      <c r="E7">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F7" s="3">
-        <v>0.26500000000000001</v>
-      </c>
-      <c r="G7" s="3">
-        <v>0.28199999999999997</v>
+      <c r="F7">
+        <v>0.23</v>
+      </c>
+      <c r="G7">
+        <v>0.247</v>
       </c>
       <c r="J7" s="3"/>
       <c r="L7" s="4"/>
@@ -3576,27 +3879,27 @@
       <c r="O7" s="3"/>
       <c r="P7" s="3"/>
     </row>
-    <row r="8" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>29</v>
       </c>
       <c r="B8" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="4">
-        <v>2.2650000000000002E-5</v>
-      </c>
-      <c r="D8" s="4">
-        <v>8.8139999999999996E-4</v>
-      </c>
-      <c r="E8" s="4">
+      <c r="C8">
+        <v>2.4110000000000001E-5</v>
+      </c>
+      <c r="D8">
+        <v>8.8170000000000002E-4</v>
+      </c>
+      <c r="E8">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F8" s="3">
-        <v>0.29399999999999998</v>
-      </c>
-      <c r="G8" s="3">
-        <v>0.32100000000000001</v>
+      <c r="F8">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="G8">
+        <v>0.28299999999999997</v>
       </c>
       <c r="J8" s="3"/>
       <c r="L8" s="4"/>
@@ -3605,27 +3908,27 @@
       <c r="O8" s="3"/>
       <c r="P8" s="3"/>
     </row>
-    <row r="9" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B9" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="4">
-        <v>7.8960000000000004E-34</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C9">
+        <v>6.2109999999999996E-34</v>
+      </c>
+      <c r="D9">
         <v>1.4249999999999999E-4</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F9" s="3">
-        <v>0.58699999999999997</v>
-      </c>
-      <c r="G9" s="3">
-        <v>0.61099999999999999</v>
+      <c r="F9">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.54700000000000004</v>
       </c>
       <c r="J9" s="3"/>
       <c r="L9" s="4"/>
@@ -3634,27 +3937,27 @@
       <c r="O9" s="3"/>
       <c r="P9" s="3"/>
     </row>
-    <row r="10" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B10" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="4">
-        <v>2.7439999999999999E-34</v>
-      </c>
-      <c r="D10" s="4">
+      <c r="C10">
+        <v>7.7039999999999993E-34</v>
+      </c>
+      <c r="D10">
         <v>1.4119999999999999E-4</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F10" s="3">
-        <v>0.999</v>
-      </c>
-      <c r="G10" s="3">
-        <v>1.036</v>
+      <c r="F10">
+        <v>0.96699999999999997</v>
+      </c>
+      <c r="G10">
+        <v>0.94399999999999995</v>
       </c>
       <c r="J10" s="3"/>
       <c r="L10" s="4"/>
@@ -3663,27 +3966,27 @@
       <c r="O10" s="3"/>
       <c r="P10" s="3"/>
     </row>
-    <row r="11" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B11" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="4">
-        <v>8.4740000000000008E-34</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1.407E-4</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="C11">
+        <v>1.1030000000000001E-33</v>
+      </c>
+      <c r="D11">
+        <v>1.4090000000000001E-4</v>
+      </c>
+      <c r="E11">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F11" s="3">
-        <v>1.9379999999999999</v>
-      </c>
-      <c r="G11" s="3">
-        <v>2.0019999999999998</v>
+      <c r="F11">
+        <v>1.716</v>
+      </c>
+      <c r="G11">
+        <v>1.738</v>
       </c>
       <c r="J11" s="3"/>
       <c r="L11" s="4"/>
@@ -3692,27 +3995,27 @@
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
     </row>
-    <row r="12" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="4">
-        <v>8.4740000000000008E-34</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1.416E-4</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="C12">
+        <v>8.9070000000000001E-34</v>
+      </c>
+      <c r="D12">
+        <v>1.4190000000000001E-4</v>
+      </c>
+      <c r="E12">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F12" s="3">
-        <v>1.198</v>
-      </c>
-      <c r="G12" s="3">
-        <v>1.2</v>
+      <c r="F12">
+        <v>1.1040000000000001</v>
+      </c>
+      <c r="G12">
+        <v>1.107</v>
       </c>
       <c r="J12" s="3"/>
       <c r="L12" s="4"/>
@@ -3721,27 +4024,27 @@
       <c r="O12" s="3"/>
       <c r="P12" s="3"/>
     </row>
-    <row r="13" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="4">
-        <v>1.5209999999999999E-33</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.3540000000000001E-4</v>
-      </c>
-      <c r="E13" s="4">
+      <c r="C13">
+        <v>7.5109999999999996E-34</v>
+      </c>
+      <c r="D13">
+        <v>1.3630000000000001E-4</v>
+      </c>
+      <c r="E13">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F13" s="3">
-        <v>1.1870000000000001</v>
-      </c>
-      <c r="G13" s="3">
-        <v>1.2190000000000001</v>
+      <c r="F13">
+        <v>1.056</v>
+      </c>
+      <c r="G13">
+        <v>1.0920000000000001</v>
       </c>
       <c r="J13" s="3"/>
       <c r="L13" s="4"/>
@@ -3750,27 +4053,27 @@
       <c r="O13" s="3"/>
       <c r="P13" s="3"/>
     </row>
-    <row r="14" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4">
-        <v>8.9359999999999997E-33</v>
-      </c>
-      <c r="D14" s="4">
+      <c r="C14">
+        <v>1.9719999999999999E-32</v>
+      </c>
+      <c r="D14">
         <v>8.0110000000000008E-3</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F14" s="3">
-        <v>0.26900000000000002</v>
-      </c>
-      <c r="G14" s="3">
-        <v>0.27200000000000002</v>
+      <c r="F14">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G14">
+        <v>3.9E-2</v>
       </c>
       <c r="J14" s="3"/>
       <c r="L14" s="4"/>
@@ -3779,27 +4082,27 @@
       <c r="O14" s="3"/>
       <c r="P14" s="3"/>
     </row>
-    <row r="15" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="4">
-        <v>9.5530000000000003E-33</v>
-      </c>
-      <c r="D15" s="4">
+      <c r="C15">
+        <v>1.5409999999999999E-32</v>
+      </c>
+      <c r="D15">
         <v>7.7460000000000003E-3</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F15" s="3">
-        <v>1.728</v>
-      </c>
-      <c r="G15" s="3">
-        <v>1.76</v>
+      <c r="F15">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="G15">
+        <v>0.107</v>
       </c>
       <c r="J15" s="3"/>
       <c r="L15" s="4"/>
@@ -3808,27 +4111,27 @@
       <c r="O15" s="3"/>
       <c r="P15" s="3"/>
     </row>
-    <row r="16" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B16" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="4">
-        <v>7.396E-33</v>
-      </c>
-      <c r="D16" s="4">
+      <c r="C16">
+        <v>9.5530000000000003E-33</v>
+      </c>
+      <c r="D16">
         <v>7.8510000000000003E-3</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F16" s="3">
-        <v>1.7989999999999999</v>
-      </c>
-      <c r="G16" s="3">
-        <v>1.8460000000000001</v>
+      <c r="F16">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="G16">
+        <v>0.185</v>
       </c>
       <c r="J16" s="3"/>
       <c r="L16" s="4"/>
@@ -3837,27 +4140,27 @@
       <c r="O16" s="3"/>
       <c r="P16" s="3"/>
     </row>
-    <row r="17" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="4">
-        <v>1.1400000000000001E-32</v>
-      </c>
-      <c r="D17" s="4">
+      <c r="C17">
+        <v>1.079E-32</v>
+      </c>
+      <c r="D17">
         <v>7.8919999999999997E-3</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F17" s="3">
-        <v>1.849</v>
-      </c>
-      <c r="G17" s="3">
-        <v>1.909</v>
+      <c r="F17">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="G17">
+        <v>0.27300000000000002</v>
       </c>
       <c r="J17" s="3"/>
       <c r="L17" s="4"/>
@@ -3866,27 +4169,27 @@
       <c r="O17" s="3"/>
       <c r="P17" s="3"/>
     </row>
-    <row r="18" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B18" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="4">
-        <v>8.0119999999999999E-33</v>
-      </c>
-      <c r="D18" s="4">
+      <c r="C18">
+        <v>1.7560000000000001E-32</v>
+      </c>
+      <c r="D18">
         <v>7.2789999999999999E-3</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F18" s="3">
-        <v>1.0049999999999999</v>
-      </c>
-      <c r="G18" s="3">
-        <v>1.0489999999999999</v>
+      <c r="F18">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="G18">
+        <v>0.34799999999999998</v>
       </c>
       <c r="J18" s="3"/>
       <c r="L18" s="4"/>
@@ -3895,27 +4198,27 @@
       <c r="O18" s="3"/>
       <c r="P18" s="3"/>
     </row>
-    <row r="19" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>13</v>
       </c>
-      <c r="C19" s="4">
-        <v>2.0410000000000001E-33</v>
-      </c>
-      <c r="D19" s="4">
+      <c r="C19">
+        <v>2.1760000000000002E-33</v>
+      </c>
+      <c r="D19">
         <v>2.0539999999999998E-3</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F19" s="3">
-        <v>0.4</v>
-      </c>
-      <c r="G19" s="3">
-        <v>0.39700000000000002</v>
+      <c r="F19">
+        <v>6.3E-2</v>
+      </c>
+      <c r="G19">
+        <v>5.5E-2</v>
       </c>
       <c r="J19" s="3"/>
       <c r="L19" s="4"/>
@@ -3924,27 +4227,27 @@
       <c r="O19" s="3"/>
       <c r="P19" s="3"/>
     </row>
-    <row r="20" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="4">
-        <v>2.215E-33</v>
-      </c>
-      <c r="D20" s="4">
+      <c r="C20">
+        <v>2.5040000000000001E-33</v>
+      </c>
+      <c r="D20">
         <v>2.0010000000000002E-3</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F20" s="3">
-        <v>2.452</v>
-      </c>
-      <c r="G20" s="3">
-        <v>2.4239999999999999</v>
+      <c r="F20">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="G20">
+        <v>0.159</v>
       </c>
       <c r="J20" s="3"/>
       <c r="L20" s="4"/>
@@ -3953,27 +4256,27 @@
       <c r="O20" s="3"/>
       <c r="P20" s="3"/>
     </row>
-    <row r="21" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="4">
-        <v>3.0429999999999999E-33</v>
-      </c>
-      <c r="D21" s="4">
+      <c r="C21">
+        <v>1.6369999999999999E-33</v>
+      </c>
+      <c r="D21">
         <v>2.042E-3</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F21" s="3">
-        <v>2.5339999999999998</v>
-      </c>
-      <c r="G21" s="3">
-        <v>2.4849999999999999</v>
+      <c r="F21">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="G21">
+        <v>0.21099999999999999</v>
       </c>
       <c r="J21" s="3"/>
       <c r="L21" s="4"/>
@@ -3982,27 +4285,27 @@
       <c r="O21" s="3"/>
       <c r="P21" s="3"/>
     </row>
-    <row r="22" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B22" t="s">
         <v>11</v>
       </c>
-      <c r="C22" s="4">
-        <v>1.8100000000000001E-33</v>
-      </c>
-      <c r="D22" s="4">
+      <c r="C22">
+        <v>2.812E-33</v>
+      </c>
+      <c r="D22">
         <v>2.0309999999999998E-3</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F22" s="3">
-        <v>2.613</v>
-      </c>
-      <c r="G22" s="3">
-        <v>2.5659999999999998</v>
+      <c r="F22">
+        <v>0.308</v>
+      </c>
+      <c r="G22">
+        <v>0.30399999999999999</v>
       </c>
       <c r="J22" s="3"/>
       <c r="L22" s="4"/>
@@ -4011,27 +4314,27 @@
       <c r="O22" s="3"/>
       <c r="P22" s="3"/>
     </row>
-    <row r="23" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B23" t="s">
         <v>12</v>
       </c>
-      <c r="C23" s="4">
-        <v>5.7780000000000003E-34</v>
-      </c>
-      <c r="D23" s="4">
+      <c r="C23">
+        <v>1.9070000000000001E-33</v>
+      </c>
+      <c r="D23">
         <v>1.812E-3</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F23" s="3">
-        <v>1.39</v>
-      </c>
-      <c r="G23" s="3">
-        <v>1.397</v>
+      <c r="F23">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.378</v>
       </c>
       <c r="J23" s="3"/>
       <c r="L23" s="4"/>
@@ -4040,27 +4343,27 @@
       <c r="O23" s="3"/>
       <c r="P23" s="3"/>
     </row>
-    <row r="24" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B24" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="4">
-        <v>2.2200000000000002E-3</v>
-      </c>
-      <c r="D24" s="4">
-        <v>3.4270000000000002E-2</v>
-      </c>
-      <c r="E24" s="4">
+      <c r="C24">
+        <v>2.7360000000000002E-3</v>
+      </c>
+      <c r="D24">
+        <v>3.465E-2</v>
+      </c>
+      <c r="E24">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F24" s="3">
-        <v>0.61399999999999999</v>
-      </c>
-      <c r="G24" s="3">
-        <v>0.624</v>
+      <c r="F24">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="G24">
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="J24" s="3"/>
       <c r="L24" s="4"/>
@@ -4069,27 +4372,27 @@
       <c r="O24" s="3"/>
       <c r="P24" s="3"/>
     </row>
-    <row r="25" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B25" t="s">
         <v>9</v>
       </c>
-      <c r="C25" s="4">
-        <v>3.1359999999999999E-3</v>
-      </c>
-      <c r="D25" s="4">
-        <v>2.9610000000000001E-2</v>
-      </c>
-      <c r="E25" s="4">
+      <c r="C25">
+        <v>3.5999999999999999E-3</v>
+      </c>
+      <c r="D25">
+        <v>3.023E-2</v>
+      </c>
+      <c r="E25">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F25" s="3">
-        <v>1.8380000000000001</v>
-      </c>
-      <c r="G25" s="3">
-        <v>1.89</v>
+      <c r="F25">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G25">
+        <v>0.154</v>
       </c>
       <c r="J25" s="3"/>
       <c r="L25" s="4"/>
@@ -4098,27 +4401,27 @@
       <c r="O25" s="3"/>
       <c r="P25" s="3"/>
     </row>
-    <row r="26" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B26" t="s">
         <v>10</v>
       </c>
-      <c r="C26" s="4">
-        <v>2.2239999999999998E-3</v>
-      </c>
-      <c r="D26" s="4">
-        <v>3.8109999999999998E-2</v>
-      </c>
-      <c r="E26" s="4">
+      <c r="C26">
+        <v>2.7560000000000002E-3</v>
+      </c>
+      <c r="D26">
+        <v>3.8449999999999998E-2</v>
+      </c>
+      <c r="E26">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F26" s="3">
-        <v>1.8839999999999999</v>
-      </c>
-      <c r="G26" s="3">
-        <v>1.9470000000000001</v>
+      <c r="F26">
+        <v>0.23</v>
+      </c>
+      <c r="G26">
+        <v>0.25</v>
       </c>
       <c r="J26" s="3"/>
       <c r="L26" s="4"/>
@@ -4127,27 +4430,27 @@
       <c r="O26" s="3"/>
       <c r="P26" s="3"/>
     </row>
-    <row r="27" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B27" t="s">
         <v>11</v>
       </c>
-      <c r="C27" s="4">
-        <v>2.3730000000000001E-3</v>
-      </c>
-      <c r="D27" s="4">
-        <v>3.9269999999999999E-2</v>
-      </c>
-      <c r="E27" s="4">
+      <c r="C27">
+        <v>2.689E-3</v>
+      </c>
+      <c r="D27">
+        <v>4.0140000000000002E-2</v>
+      </c>
+      <c r="E27">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F27" s="3">
-        <v>1.954</v>
-      </c>
-      <c r="G27" s="3">
-        <v>2.0350000000000001</v>
+      <c r="F27">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="G27">
+        <v>0.316</v>
       </c>
       <c r="J27" s="3"/>
       <c r="L27" s="4"/>
@@ -4156,27 +4459,27 @@
       <c r="O27" s="3"/>
       <c r="P27" s="3"/>
     </row>
-    <row r="28" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="4">
-        <v>2.3400000000000001E-3</v>
-      </c>
-      <c r="D28" s="4">
-        <v>3.0929999999999999E-2</v>
-      </c>
-      <c r="E28" s="4">
+      <c r="C28">
+        <v>2.921E-3</v>
+      </c>
+      <c r="D28">
+        <v>3.116E-2</v>
+      </c>
+      <c r="E28">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F28" s="3">
-        <v>1.456</v>
-      </c>
-      <c r="G28" s="3">
-        <v>1.4990000000000001</v>
+      <c r="F28">
+        <v>0.371</v>
+      </c>
+      <c r="G28">
+        <v>0.41099999999999998</v>
       </c>
       <c r="J28" s="3"/>
       <c r="L28" s="4"/>
@@ -4185,27 +4488,27 @@
       <c r="O28" s="3"/>
       <c r="P28" s="3"/>
     </row>
-    <row r="29" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B29" t="s">
         <v>13</v>
       </c>
-      <c r="C29" s="4">
-        <v>2.6719999999999999E-3</v>
-      </c>
-      <c r="D29" s="4">
-        <v>1.259E-2</v>
-      </c>
-      <c r="E29" s="4">
+      <c r="C29">
+        <v>2.555E-3</v>
+      </c>
+      <c r="D29">
+        <v>1.2319999999999999E-2</v>
+      </c>
+      <c r="E29">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F29" s="3">
-        <v>0.88</v>
-      </c>
-      <c r="G29" s="3">
-        <v>0.86</v>
+      <c r="F29">
+        <v>9.4E-2</v>
+      </c>
+      <c r="G29">
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="J29" s="3"/>
       <c r="L29" s="4"/>
@@ -4214,27 +4517,27 @@
       <c r="O29" s="3"/>
       <c r="P29" s="3"/>
     </row>
-    <row r="30" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>9</v>
       </c>
-      <c r="C30" s="4">
-        <v>2.7490000000000001E-3</v>
-      </c>
-      <c r="D30" s="4">
-        <v>1.128E-2</v>
-      </c>
-      <c r="E30" s="4">
+      <c r="C30">
+        <v>2.7320000000000001E-3</v>
+      </c>
+      <c r="D30">
+        <v>1.1730000000000001E-2</v>
+      </c>
+      <c r="E30">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F30" s="3">
-        <v>2.64</v>
-      </c>
-      <c r="G30" s="3">
-        <v>2.5910000000000002</v>
+      <c r="F30">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G30">
+        <v>0.19700000000000001</v>
       </c>
       <c r="J30" s="3"/>
       <c r="L30" s="4"/>
@@ -4243,27 +4546,27 @@
       <c r="O30" s="3"/>
       <c r="P30" s="3"/>
     </row>
-    <row r="31" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>10</v>
       </c>
-      <c r="C31" s="4">
-        <v>2.0990000000000002E-3</v>
-      </c>
-      <c r="D31" s="4">
-        <v>1.438E-2</v>
-      </c>
-      <c r="E31" s="4">
+      <c r="C31">
+        <v>2.0660000000000001E-3</v>
+      </c>
+      <c r="D31">
+        <v>1.519E-2</v>
+      </c>
+      <c r="E31">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F31" s="3">
-        <v>2.6909999999999998</v>
-      </c>
-      <c r="G31" s="3">
-        <v>2.6419999999999999</v>
+      <c r="F31">
+        <v>0.255</v>
+      </c>
+      <c r="G31">
+        <v>0.25900000000000001</v>
       </c>
       <c r="J31" s="3"/>
       <c r="L31" s="4"/>
@@ -4272,27 +4575,27 @@
       <c r="O31" s="3"/>
       <c r="P31" s="3"/>
     </row>
-    <row r="32" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B32" t="s">
         <v>11</v>
       </c>
-      <c r="C32" s="4">
-        <v>2.2920000000000002E-3</v>
-      </c>
-      <c r="D32" s="4">
-        <v>1.5720000000000001E-2</v>
-      </c>
-      <c r="E32" s="4">
+      <c r="C32">
+        <v>2.0730000000000002E-3</v>
+      </c>
+      <c r="D32">
+        <v>1.5859999999999999E-2</v>
+      </c>
+      <c r="E32">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F32" s="3">
-        <v>2.7570000000000001</v>
-      </c>
-      <c r="G32" s="3">
-        <v>2.73</v>
+      <c r="F32">
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="G32">
+        <v>0.34</v>
       </c>
       <c r="J32" s="3"/>
       <c r="L32" s="4"/>
@@ -4301,27 +4604,27 @@
       <c r="O32" s="3"/>
       <c r="P32" s="3"/>
     </row>
-    <row r="33" spans="1:16" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:16" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B33" t="s">
         <v>12</v>
       </c>
-      <c r="C33" s="4">
-        <v>4.2950000000000002E-3</v>
-      </c>
-      <c r="D33" s="4">
-        <v>9.9760000000000005E-3</v>
-      </c>
-      <c r="E33" s="4">
+      <c r="C33">
+        <v>4.1240000000000001E-3</v>
+      </c>
+      <c r="D33">
+        <v>9.3150000000000004E-3</v>
+      </c>
+      <c r="E33">
         <v>9.0690000000000001E-5</v>
       </c>
-      <c r="F33" s="3">
-        <v>1.962</v>
-      </c>
-      <c r="G33" s="3">
-        <v>1.927</v>
+      <c r="F33">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="G33">
+        <v>0.434</v>
       </c>
       <c r="J33" s="3"/>
       <c r="L33" s="4"/>

</xml_diff>